<commit_message>
Updated template for to add "Wet" effects
</commit_message>
<xml_diff>
--- a/public/excel template/Template.xlsx
+++ b/public/excel template/Template.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="202300"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B0FAB3F-9CE8-4F8D-B8FB-BFF4EB8620E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADADAFDD-440A-42BD-93B4-A2237623D618}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27825" yWindow="1515" windowWidth="16485" windowHeight="13440" xr2:uid="{BECE5613-4CE6-4BB7-8FF1-F4E60925457F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BECE5613-4CE6-4BB7-8FF1-F4E60925457F}"/>
   </bookViews>
   <sheets>
     <sheet name="Small" sheetId="2" r:id="rId1"/>
@@ -572,7 +572,70 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="13">
+    <dxf>
+      <fill>
+        <patternFill patternType="gray125"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightGray"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightGray"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightGray"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightGray"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightGray"/>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -951,7 +1014,7 @@
   <dimension ref="A1:Z18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1041,11 +1104,11 @@
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
       <c r="J5" s="38">
-        <v>45734</v>
+        <v>45825</v>
       </c>
       <c r="K5" s="38">
         <f>J5+6</f>
-        <v>45740</v>
+        <v>45831</v>
       </c>
       <c r="M5" s="13"/>
       <c r="N5" s="13"/>
@@ -1074,11 +1137,11 @@
       <c r="I6" s="15"/>
       <c r="J6" s="35">
         <f>J5+7</f>
-        <v>45741</v>
+        <v>45832</v>
       </c>
       <c r="K6" s="35">
         <f>K5+7</f>
-        <v>45747</v>
+        <v>45838</v>
       </c>
       <c r="M6" s="13"/>
       <c r="N6" s="16"/>
@@ -1108,11 +1171,11 @@
       <c r="I7" s="10"/>
       <c r="J7" s="35">
         <f t="shared" ref="J7:K16" si="0">J6+7</f>
-        <v>45748</v>
+        <v>45839</v>
       </c>
       <c r="K7" s="35">
         <f t="shared" si="0"/>
-        <v>45754</v>
+        <v>45845</v>
       </c>
       <c r="M7" s="13"/>
       <c r="N7" s="17"/>
@@ -1143,11 +1206,11 @@
       <c r="I8" s="10"/>
       <c r="J8" s="35">
         <f t="shared" si="0"/>
-        <v>45755</v>
+        <v>45846</v>
       </c>
       <c r="K8" s="35">
         <f t="shared" si="0"/>
-        <v>45761</v>
+        <v>45852</v>
       </c>
       <c r="M8" s="13"/>
       <c r="N8" s="19"/>
@@ -1171,11 +1234,11 @@
       <c r="I9" s="10"/>
       <c r="J9" s="35">
         <f t="shared" si="0"/>
-        <v>45762</v>
+        <v>45853</v>
       </c>
       <c r="K9" s="35">
         <f t="shared" si="0"/>
-        <v>45768</v>
+        <v>45859</v>
       </c>
       <c r="M9" s="13"/>
       <c r="N9" s="17"/>
@@ -1199,11 +1262,11 @@
       <c r="I10" s="10"/>
       <c r="J10" s="35">
         <f t="shared" si="0"/>
-        <v>45769</v>
+        <v>45860</v>
       </c>
       <c r="K10" s="35">
         <f t="shared" si="0"/>
-        <v>45775</v>
+        <v>45866</v>
       </c>
       <c r="M10" s="13"/>
       <c r="N10" s="17"/>
@@ -1227,11 +1290,11 @@
       <c r="I11" s="10"/>
       <c r="J11" s="35">
         <f t="shared" si="0"/>
-        <v>45776</v>
+        <v>45867</v>
       </c>
       <c r="K11" s="35">
         <f t="shared" si="0"/>
-        <v>45782</v>
+        <v>45873</v>
       </c>
       <c r="M11" s="13"/>
       <c r="N11" s="17"/>
@@ -1255,11 +1318,11 @@
       <c r="I12" s="10"/>
       <c r="J12" s="35">
         <f t="shared" si="0"/>
-        <v>45783</v>
+        <v>45874</v>
       </c>
       <c r="K12" s="35">
         <f t="shared" si="0"/>
-        <v>45789</v>
+        <v>45880</v>
       </c>
       <c r="M12" s="13"/>
       <c r="N12" s="17"/>
@@ -1283,11 +1346,11 @@
       <c r="I13" s="10"/>
       <c r="J13" s="35">
         <f t="shared" si="0"/>
-        <v>45790</v>
+        <v>45881</v>
       </c>
       <c r="K13" s="35">
         <f t="shared" si="0"/>
-        <v>45796</v>
+        <v>45887</v>
       </c>
       <c r="M13" s="13"/>
       <c r="N13" s="17"/>
@@ -1311,11 +1374,11 @@
       <c r="I14" s="10"/>
       <c r="J14" s="35">
         <f t="shared" si="0"/>
-        <v>45797</v>
+        <v>45888</v>
       </c>
       <c r="K14" s="35">
         <f t="shared" si="0"/>
-        <v>45803</v>
+        <v>45894</v>
       </c>
       <c r="M14" s="13"/>
       <c r="N14" s="17"/>
@@ -1339,11 +1402,11 @@
       <c r="I15" s="10"/>
       <c r="J15" s="35">
         <f t="shared" si="0"/>
-        <v>45804</v>
+        <v>45895</v>
       </c>
       <c r="K15" s="35">
         <f t="shared" si="0"/>
-        <v>45810</v>
+        <v>45901</v>
       </c>
       <c r="M15" s="13"/>
       <c r="N15" s="17"/>
@@ -1367,11 +1430,11 @@
       <c r="I16" s="22"/>
       <c r="J16" s="52">
         <f t="shared" si="0"/>
-        <v>45811</v>
+        <v>45902</v>
       </c>
       <c r="K16" s="52">
         <f t="shared" si="0"/>
-        <v>45817</v>
+        <v>45908</v>
       </c>
       <c r="M16" s="13"/>
       <c r="N16" s="17"/>
@@ -1403,14 +1466,9 @@
       <c r="T18" s="17"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A4:L4 J17">
-    <cfRule type="expression" dxfId="3" priority="1">
-      <formula>$K4="Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A5:L16">
-    <cfRule type="expression" dxfId="2" priority="4">
-      <formula>$L5="Yes"</formula>
+  <conditionalFormatting sqref="B5:I16">
+    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="%">
+      <formula>NOT(ISERROR(SEARCH("%",B5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -1424,8 +1482,8 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:EV18"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="EF6" sqref="EF6"/>
+    <sheetView topLeftCell="DV1" workbookViewId="0">
+      <selection activeCell="EB9" sqref="EB9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2137,11 +2195,11 @@
       <c r="ED5" s="10"/>
       <c r="EE5" s="10"/>
       <c r="EF5" s="11">
-        <v>45734</v>
+        <v>45825</v>
       </c>
       <c r="EG5" s="12">
         <f>EF5+6</f>
-        <v>45740</v>
+        <v>45831</v>
       </c>
       <c r="EI5" s="13"/>
       <c r="EJ5" s="13"/>
@@ -2296,11 +2354,11 @@
       <c r="EE6" s="10"/>
       <c r="EF6" s="11">
         <f>EF5+7</f>
-        <v>45741</v>
+        <v>45832</v>
       </c>
       <c r="EG6" s="12">
         <f>EG5+7</f>
-        <v>45747</v>
+        <v>45838</v>
       </c>
       <c r="EI6" s="13"/>
       <c r="EJ6" s="16"/>
@@ -2456,11 +2514,11 @@
       <c r="EE7" s="10"/>
       <c r="EF7" s="11">
         <f t="shared" ref="EF7:EG16" si="0">EF6+7</f>
-        <v>45748</v>
+        <v>45839</v>
       </c>
       <c r="EG7" s="12">
         <f t="shared" si="0"/>
-        <v>45754</v>
+        <v>45845</v>
       </c>
       <c r="EI7" s="13"/>
       <c r="EJ7" s="17"/>
@@ -2617,11 +2675,11 @@
       <c r="EE8" s="10"/>
       <c r="EF8" s="11">
         <f t="shared" si="0"/>
-        <v>45755</v>
+        <v>45846</v>
       </c>
       <c r="EG8" s="12">
         <f t="shared" si="0"/>
-        <v>45761</v>
+        <v>45852</v>
       </c>
       <c r="EI8" s="13"/>
       <c r="EJ8" s="19"/>
@@ -2771,11 +2829,11 @@
       <c r="EE9" s="10"/>
       <c r="EF9" s="11">
         <f t="shared" si="0"/>
-        <v>45762</v>
+        <v>45853</v>
       </c>
       <c r="EG9" s="12">
         <f t="shared" si="0"/>
-        <v>45768</v>
+        <v>45859</v>
       </c>
       <c r="EI9" s="13"/>
       <c r="EJ9" s="17"/>
@@ -2925,11 +2983,11 @@
       <c r="EE10" s="10"/>
       <c r="EF10" s="11">
         <f t="shared" si="0"/>
-        <v>45769</v>
+        <v>45860</v>
       </c>
       <c r="EG10" s="12">
         <f t="shared" si="0"/>
-        <v>45775</v>
+        <v>45866</v>
       </c>
       <c r="EI10" s="13"/>
       <c r="EJ10" s="17"/>
@@ -3079,11 +3137,11 @@
       <c r="EE11" s="10"/>
       <c r="EF11" s="11">
         <f t="shared" si="0"/>
-        <v>45776</v>
+        <v>45867</v>
       </c>
       <c r="EG11" s="12">
         <f t="shared" si="0"/>
-        <v>45782</v>
+        <v>45873</v>
       </c>
       <c r="EI11" s="13"/>
       <c r="EJ11" s="17"/>
@@ -3233,11 +3291,11 @@
       <c r="EE12" s="10"/>
       <c r="EF12" s="11">
         <f t="shared" si="0"/>
-        <v>45783</v>
+        <v>45874</v>
       </c>
       <c r="EG12" s="12">
         <f t="shared" si="0"/>
-        <v>45789</v>
+        <v>45880</v>
       </c>
       <c r="EI12" s="13"/>
       <c r="EJ12" s="17"/>
@@ -3387,11 +3445,11 @@
       <c r="EE13" s="10"/>
       <c r="EF13" s="11">
         <f t="shared" si="0"/>
-        <v>45790</v>
+        <v>45881</v>
       </c>
       <c r="EG13" s="12">
         <f t="shared" si="0"/>
-        <v>45796</v>
+        <v>45887</v>
       </c>
       <c r="EI13" s="13"/>
       <c r="EJ13" s="17"/>
@@ -3541,11 +3599,11 @@
       <c r="EE14" s="10"/>
       <c r="EF14" s="11">
         <f t="shared" si="0"/>
-        <v>45797</v>
+        <v>45888</v>
       </c>
       <c r="EG14" s="12">
         <f t="shared" si="0"/>
-        <v>45803</v>
+        <v>45894</v>
       </c>
       <c r="EI14" s="13"/>
       <c r="EJ14" s="17"/>
@@ -3695,11 +3753,11 @@
       <c r="EE15" s="10"/>
       <c r="EF15" s="11">
         <f t="shared" si="0"/>
-        <v>45804</v>
+        <v>45895</v>
       </c>
       <c r="EG15" s="12">
         <f t="shared" si="0"/>
-        <v>45810</v>
+        <v>45901</v>
       </c>
       <c r="EI15" s="13"/>
       <c r="EJ15" s="17"/>
@@ -3849,11 +3907,11 @@
       <c r="EE16" s="22"/>
       <c r="EF16" s="11">
         <f t="shared" si="0"/>
-        <v>45811</v>
+        <v>45902</v>
       </c>
       <c r="EG16" s="12">
         <f t="shared" si="0"/>
-        <v>45817</v>
+        <v>45908</v>
       </c>
       <c r="EI16" s="13"/>
       <c r="EJ16" s="17"/>
@@ -3884,14 +3942,9 @@
       <c r="EP18" s="17"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A4:EG4">
-    <cfRule type="expression" dxfId="1" priority="1">
-      <formula>$EG4="Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A5:EH16">
-    <cfRule type="expression" dxfId="0" priority="5">
-      <formula>$EH5="Yes"</formula>
+  <conditionalFormatting sqref="B5:EE16">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="%">
+      <formula>NOT(ISERROR(SEARCH("%",B5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.2" right="0.2" top="0.4" bottom="0.4" header="0.3" footer="0.3"/>

</xml_diff>